<commit_message>
adding in some inital analyses with preprocessing of 7 day data
</commit_message>
<xml_diff>
--- a/data/pilot/7 days/06062023 salbutamol pilot fish metadata.xlsx
+++ b/data/pilot/7 days/06062023 salbutamol pilot fish metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Box Sync/MPSIII/adult behaviour/06062023 salbutamol pilot/7 days/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Documents/2023_MPSIII_salbutamol/data/pilot/7 days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4566A2C6-AD11-E640-99F7-1AB7BEB084D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89AF05C-3EC0-2D43-83B4-2CF72941EAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28240" yWindow="-2340" windowWidth="23320" windowHeight="18220" xr2:uid="{C9C2347C-DF6E-2E45-B61F-0188AEE3841E}"/>
+    <workbookView xWindow="25880" yWindow="-11500" windowWidth="20140" windowHeight="19360" xr2:uid="{C9C2347C-DF6E-2E45-B61F-0188AEE3841E}"/>
   </bookViews>
   <sheets>
     <sheet name="7 days" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="45">
   <si>
     <t>fish_id</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>YMaze_tracking-20230606T154117-f30.avi</t>
+  </si>
+  <si>
+    <t>data_file_zones</t>
+  </si>
+  <si>
+    <t>data_file_distances</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230606T115219-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230606T130410-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230606T141945-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230606T153443-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230606T115516-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230606T130748-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230606T142314-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230606T154046-data_totals.csv</t>
   </si>
 </sst>
 </file>
@@ -268,7 +298,489 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="60">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -291,309 +803,6 @@
     <dxf>
       <fill>
         <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
@@ -736,196 +945,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -940,34 +959,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53A38344-3126-814D-B750-1D7313E7AC91}" name="Table1" displayName="Table1" ref="A1:J60" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40">
-  <autoFilter ref="A1:J60" xr:uid="{14BEAE75-E040-A249-8390-C6C592CA9991}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{83EFEAF9-8016-B14F-A240-1D31C677A829}" name="fish_id" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{5B1A58C4-4FA4-F040-A213-F632490B715A}" name="treatment" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{D17F91BA-89B1-6840-AC8D-3BEE4A72BE77}" name="sex" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{B386D8A1-5336-454D-B2F5-B48299CDC626}" name="start time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{2B963070-35AB-1D41-AB37-8CD88D3AD7AB}" name="ymazeUnit" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{2A356590-AC74-5242-8339-6FCE3FFD0E34}" name="ymazePosition" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{68688BAB-7BE6-5948-8E11-EC7CCD978351}" name="data_file" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{F394C5A6-BD4A-9B4D-8D1D-276E13DE473C}" name="videoFile" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{12BB17E8-5F27-724E-ACEA-3B58E4A5D42B}" name="Comment" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{97D2480A-9982-3B4C-AA40-6541F57274D0}" name="genotype" dataDxfId="29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53A38344-3126-814D-B750-1D7313E7AC91}" name="Table1" displayName="Table1" ref="A1:K60" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58">
+  <autoFilter ref="A1:K60" xr:uid="{14BEAE75-E040-A249-8390-C6C592CA9991}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{83EFEAF9-8016-B14F-A240-1D31C677A829}" name="fish_id" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{5B1A58C4-4FA4-F040-A213-F632490B715A}" name="treatment" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{D17F91BA-89B1-6840-AC8D-3BEE4A72BE77}" name="sex" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{B386D8A1-5336-454D-B2F5-B48299CDC626}" name="start time" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{2B963070-35AB-1D41-AB37-8CD88D3AD7AB}" name="ymazeUnit" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{2A356590-AC74-5242-8339-6FCE3FFD0E34}" name="ymazePosition" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{69EE2184-8E68-0B4C-9C0D-F7E1B7B14DC2}" name="data_file_distances" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{68688BAB-7BE6-5948-8E11-EC7CCD978351}" name="data_file_zones" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{F394C5A6-BD4A-9B4D-8D1D-276E13DE473C}" name="videoFile" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{12BB17E8-5F27-724E-ACEA-3B58E4A5D42B}" name="Comment" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{97D2480A-9982-3B4C-AA40-6541F57274D0}" name="genotype" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C873B688-B02F-3841-9AC9-DB63D3D6D6E4}" name="Table2" displayName="Table2" ref="A1:J60" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C873B688-B02F-3841-9AC9-DB63D3D6D6E4}" name="Table2" displayName="Table2" ref="A1:J60" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45">
   <autoFilter ref="A1:J60" xr:uid="{4A127628-89D0-2941-B704-D4C232D7D28E}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4520C07D-F5B2-3346-BFBC-BA932C91D469}" name="fish_id" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{AFB27AF1-5014-DC40-9553-64E06B3AF94E}" name="treatment" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8C8E4483-9AAC-F143-956C-E9B7B600A9B4}" name="sex" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{6D03A179-4DD6-824E-B550-083E8863CDF7}" name="start time" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6EDCB672-55D3-8944-979C-0FA58BC2098C}" name="ymazeUnit" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{71551E84-2AA1-7D4F-9E57-1F9B28E3EC5A}" name="ymazePosition" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{4520C07D-F5B2-3346-BFBC-BA932C91D469}" name="fish_id" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{AFB27AF1-5014-DC40-9553-64E06B3AF94E}" name="treatment" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{8C8E4483-9AAC-F143-956C-E9B7B600A9B4}" name="sex" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{6D03A179-4DD6-824E-B550-083E8863CDF7}" name="start time" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{6EDCB672-55D3-8944-979C-0FA58BC2098C}" name="ymazeUnit" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{71551E84-2AA1-7D4F-9E57-1F9B28E3EC5A}" name="ymazePosition" dataDxfId="39"/>
     <tableColumn id="7" xr3:uid="{DFA66FD9-F6FB-9445-AFD7-659B23A0201C}" name="data_file"/>
     <tableColumn id="8" xr3:uid="{3007FAC3-4018-0A47-8D0F-544D401DC5AD}" name="videoFile"/>
     <tableColumn id="9" xr3:uid="{9992A96B-C94F-7940-AA99-DBFF62752A53}" name="Comment"/>
@@ -1277,11 +1297,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="G54" sqref="G54:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,13 +1312,14 @@
     <col min="4" max="4" width="11.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="6.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="42.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="43.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="36.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="42.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="24.83203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,19 +1339,22 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1350,17 +1374,20 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1380,17 +1407,20 @@
         <v>2</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1410,17 +1440,20 @@
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1440,17 +1473,20 @@
         <v>4</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1470,17 +1506,20 @@
         <v>5</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1500,17 +1539,20 @@
         <v>6</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1530,17 +1572,20 @@
         <v>7</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1560,17 +1605,20 @@
         <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1589,18 +1637,21 @@
       <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1619,18 +1670,21 @@
       <c r="F11" s="5">
         <v>2</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1649,18 +1703,21 @@
       <c r="F12" s="5">
         <v>3</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1679,18 +1736,21 @@
       <c r="F13" s="5">
         <v>4</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1709,18 +1769,21 @@
       <c r="F14" s="5">
         <v>5</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1739,18 +1802,21 @@
       <c r="F15" s="5">
         <v>6</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1769,18 +1835,21 @@
       <c r="F16" s="5">
         <v>7</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="I16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1799,18 +1868,21 @@
       <c r="F17" s="5">
         <v>8</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="I17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1829,20 +1901,23 @@
       <c r="F18" s="5">
         <v>1</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1861,18 +1936,21 @@
       <c r="F19" s="5">
         <v>2</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="8" t="s">
+      <c r="I19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1891,18 +1969,21 @@
       <c r="F20" s="5">
         <v>3</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="I20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1921,18 +2002,21 @@
       <c r="F21" s="5">
         <v>4</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="4"/>
+      <c r="K21" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1951,18 +2035,21 @@
       <c r="F22" s="5">
         <v>5</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="4"/>
+      <c r="K22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1981,18 +2068,21 @@
       <c r="F23" s="5">
         <v>6</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2011,18 +2101,21 @@
       <c r="F24" s="5">
         <v>7</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2041,18 +2134,21 @@
       <c r="F25" s="5">
         <v>8</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="8" t="s">
+      <c r="I25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2071,18 +2167,21 @@
       <c r="F26" s="5">
         <v>1</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="4"/>
+      <c r="K26" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2101,20 +2200,23 @@
       <c r="F27" s="5">
         <v>2</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H27" s="4" t="s">
+      <c r="I27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="K27" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2133,18 +2235,21 @@
       <c r="F28" s="5">
         <v>3</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2163,18 +2268,21 @@
       <c r="F29" s="5">
         <v>4</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2193,18 +2301,21 @@
       <c r="F30" s="5">
         <v>5</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2223,18 +2334,21 @@
       <c r="F31" s="5">
         <v>6</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2253,18 +2367,21 @@
       <c r="F32" s="5">
         <v>7</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2283,18 +2400,21 @@
       <c r="F33" s="5">
         <v>8</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2313,18 +2433,21 @@
       <c r="F34" s="5">
         <v>1</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="I34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2343,18 +2466,21 @@
       <c r="F35" s="5">
         <v>2</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="I35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="4"/>
+      <c r="K35" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2373,18 +2499,21 @@
       <c r="F36" s="5">
         <v>3</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H36" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="I36" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2403,18 +2532,21 @@
       <c r="F37" s="5">
         <v>4</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H37" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H37" s="8" t="s">
+      <c r="I37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="4"/>
+      <c r="K37" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -2433,18 +2565,21 @@
       <c r="F38" s="5">
         <v>5</v>
       </c>
-      <c r="G38" s="8" t="s">
+      <c r="G38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H38" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="I38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4" t="s">
+      <c r="J38" s="4"/>
+      <c r="K38" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -2463,18 +2598,21 @@
       <c r="F39" s="5">
         <v>6</v>
       </c>
-      <c r="G39" s="8" t="s">
+      <c r="G39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H39" s="8" t="s">
+      <c r="I39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="4"/>
+      <c r="K39" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2493,18 +2631,21 @@
       <c r="F40" s="5">
         <v>7</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G40" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="I40" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -2523,18 +2664,21 @@
       <c r="F41" s="5">
         <v>8</v>
       </c>
-      <c r="G41" s="8" t="s">
+      <c r="G41" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H41" s="8" t="s">
+      <c r="I41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="4"/>
+      <c r="K41" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2553,18 +2697,21 @@
       <c r="F42" s="5">
         <v>1</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="I42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2583,18 +2730,21 @@
       <c r="F43" s="5">
         <v>2</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4" t="s">
+      <c r="J43" s="4"/>
+      <c r="K43" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2613,18 +2763,21 @@
       <c r="F44" s="5">
         <v>3</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G44" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="I44" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4" t="s">
+      <c r="J44" s="4"/>
+      <c r="K44" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2643,18 +2796,21 @@
       <c r="F45" s="5">
         <v>4</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H45" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="I45" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I45" s="4"/>
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="4"/>
+      <c r="K45" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2673,18 +2829,21 @@
       <c r="F46" s="5">
         <v>5</v>
       </c>
-      <c r="G46" s="8" t="s">
+      <c r="G46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H46" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="7" t="s">
+      <c r="I46" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4" t="s">
+      <c r="J46" s="4"/>
+      <c r="K46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2703,18 +2862,21 @@
       <c r="F47" s="5">
         <v>6</v>
       </c>
-      <c r="G47" s="8" t="s">
+      <c r="G47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H47" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="I47" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="4"/>
+      <c r="K47" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2733,18 +2895,21 @@
       <c r="F48" s="5">
         <v>7</v>
       </c>
-      <c r="G48" s="8" t="s">
+      <c r="G48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H48" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="I48" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="4"/>
+      <c r="K48" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2763,18 +2928,21 @@
       <c r="F49" s="5">
         <v>8</v>
       </c>
-      <c r="G49" s="8" t="s">
+      <c r="G49" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H49" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="I49" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4" t="s">
+      <c r="J49" s="4"/>
+      <c r="K49" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2793,18 +2961,21 @@
       <c r="F50" s="5">
         <v>1</v>
       </c>
-      <c r="G50" s="8" t="s">
+      <c r="G50" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H50" s="8" t="s">
+      <c r="I50" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="4"/>
+      <c r="K50" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2823,18 +2994,21 @@
       <c r="F51" s="5">
         <v>2</v>
       </c>
-      <c r="G51" s="8" t="s">
+      <c r="G51" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H51" s="8" t="s">
+      <c r="I51" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4" t="s">
+      <c r="J51" s="4"/>
+      <c r="K51" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2853,18 +3027,21 @@
       <c r="F52" s="5">
         <v>3</v>
       </c>
-      <c r="G52" s="8" t="s">
+      <c r="G52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H52" s="8" t="s">
+      <c r="I52" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4" t="s">
+      <c r="J52" s="4"/>
+      <c r="K52" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2883,18 +3060,21 @@
       <c r="F53" s="5">
         <v>4</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H53" s="8" t="s">
+      <c r="I53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="4"/>
+      <c r="K53" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2913,18 +3093,21 @@
       <c r="F54" s="5">
         <v>1</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H54" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="I54" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4" t="s">
+      <c r="J54" s="4"/>
+      <c r="K54" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2943,18 +3126,21 @@
       <c r="F55" s="5">
         <v>2</v>
       </c>
-      <c r="G55" s="8" t="s">
+      <c r="G55" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H55" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="I55" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4" t="s">
+      <c r="J55" s="4"/>
+      <c r="K55" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2973,18 +3159,21 @@
       <c r="F56" s="5">
         <v>3</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G56" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="I56" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4" t="s">
+      <c r="J56" s="4"/>
+      <c r="K56" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -3003,18 +3192,21 @@
       <c r="F57" s="5">
         <v>4</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H57" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="I57" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4" t="s">
+      <c r="J57" s="4"/>
+      <c r="K57" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -3033,18 +3225,21 @@
       <c r="F58" s="5">
         <v>5</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H58" s="7" t="s">
+      <c r="I58" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4" t="s">
+      <c r="J58" s="4"/>
+      <c r="K58" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3063,18 +3258,21 @@
       <c r="F59" s="5">
         <v>6</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="I59" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4" t="s">
+      <c r="J59" s="4"/>
+      <c r="K59" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -3093,118 +3291,121 @@
       <c r="F60" s="5">
         <v>7</v>
       </c>
-      <c r="G60" s="8" t="s">
+      <c r="G60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H60" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="I60" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="4" t="s">
+      <c r="J60" s="4"/>
+      <c r="K60" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I61"/>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J61"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H62"/>
+      <c r="K61"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I62"/>
       <c r="J62"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H63"/>
+      <c r="K62"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I63"/>
       <c r="J63"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H64"/>
+      <c r="K63"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I64"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E10:E17">
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="28" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="58" priority="31" operator="equal">
+  <conditionalFormatting sqref="K1">
+    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E49">
-    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="55" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E9">
-    <cfRule type="cellIs" dxfId="53" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E25">
-    <cfRule type="cellIs" dxfId="51" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E33">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E41">
-    <cfRule type="cellIs" dxfId="47" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:E60">
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"het"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H42" r:id="rId1" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T142344-f30.avi" xr:uid="{C5CF7AC5-E560-4F44-916A-2202C39DB532}"/>
-    <hyperlink ref="H43:H49" r:id="rId2" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T142344-f30.avi" xr:uid="{748AF394-0D76-B342-882F-46C6824FC471}"/>
-    <hyperlink ref="H54" r:id="rId3" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T154117-f30.avi" xr:uid="{751FBEB2-BC23-4D47-92FA-7AC37A6A38C7}"/>
-    <hyperlink ref="H55:H60" r:id="rId4" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T154117-f30.avi" xr:uid="{10FEF065-4774-9947-B5B1-14E246057699}"/>
+    <hyperlink ref="I42" r:id="rId1" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T142344-f30.avi" xr:uid="{C5CF7AC5-E560-4F44-916A-2202C39DB532}"/>
+    <hyperlink ref="I43:I49" r:id="rId2" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T142344-f30.avi" xr:uid="{748AF394-0D76-B342-882F-46C6824FC471}"/>
+    <hyperlink ref="I54" r:id="rId3" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T154117-f30.avi" xr:uid="{751FBEB2-BC23-4D47-92FA-7AC37A6A38C7}"/>
+    <hyperlink ref="I55:I60" r:id="rId4" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230606T154117-f30.avi" xr:uid="{10FEF065-4774-9947-B5B1-14E246057699}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="77" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4217,79 +4418,79 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"het"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E17">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E49">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E9">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E25">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E33">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E41">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:E60">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
addded salbutamol exp 1.2 data + genotyping analsysis
</commit_message>
<xml_diff>
--- a/data/pilot/7 days/06062023 salbutamol pilot fish metadata.xlsx
+++ b/data/pilot/7 days/06062023 salbutamol pilot fish metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karissabarthelson/Documents/2023_MPSIII_salbutamol/data/pilot/7 days/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89AF05C-3EC0-2D43-83B4-2CF72941EAA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC06656-4784-C745-992F-94FCA426156D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25880" yWindow="-11500" windowWidth="20140" windowHeight="19360" xr2:uid="{C9C2347C-DF6E-2E45-B61F-0188AEE3841E}"/>
+    <workbookView xWindow="26480" yWindow="-4980" windowWidth="19560" windowHeight="20980" activeTab="1" xr2:uid="{C9C2347C-DF6E-2E45-B61F-0188AEE3841E}"/>
   </bookViews>
   <sheets>
     <sheet name="7 days" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Table2[#All]</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Table1[#All]</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="73">
   <si>
     <t>fish_id</t>
   </si>
@@ -95,9 +95,6 @@
     <t>hom</t>
   </si>
   <si>
-    <t>data_file</t>
-  </si>
-  <si>
     <t>ymaze_inLT-20230606T153443.csv</t>
   </si>
   <si>
@@ -174,6 +171,93 @@
   </si>
   <si>
     <t>ymazeinLT-20230606T154046-data_totals.csv</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>small fish</t>
+  </si>
+  <si>
+    <t>behavBatch</t>
+  </si>
+  <si>
+    <t>dodgy tracking</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T104021-f30.avi</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T103951-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T103950.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T115104-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T115104.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T130222-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T130221.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T141129.csv</t>
+  </si>
+  <si>
+    <t>ymaze_inLT-20230613T141130-data_totals.csv</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T104205-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T115329-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T130533-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T141400-f30.avi</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T104135-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T104134.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T115258-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T115258.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	ymazeinLT-20230613T130503-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T130502.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T141330-data_totals.csv</t>
+  </si>
+  <si>
+    <t>ymazeinLT-20230613T141329.csv</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T115135-f30.avi</t>
+  </si>
+  <si>
+    <t>YMaze_tracking-20230613T130252-f30.avi</t>
+  </si>
+  <si>
+    <t>accidently deleted video</t>
   </si>
 </sst>
 </file>
@@ -219,7 +303,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -268,12 +352,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -293,20 +386,33 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -470,6 +576,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -687,6 +803,18 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -775,6 +903,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="1"/>
@@ -829,6 +966,15 @@
         <patternFill patternType="none">
           <fgColor theme="0" tint="-0.14999847407452621"/>
           <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -959,39 +1105,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53A38344-3126-814D-B750-1D7313E7AC91}" name="Table1" displayName="Table1" ref="A1:K60" totalsRowShown="0" headerRowDxfId="59" dataDxfId="57" headerRowBorderDxfId="58">
-  <autoFilter ref="A1:K60" xr:uid="{14BEAE75-E040-A249-8390-C6C592CA9991}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53A38344-3126-814D-B750-1D7313E7AC91}" name="Table1" displayName="Table1" ref="A1:K60" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63">
+  <autoFilter ref="A1:K60" xr:uid="{14BEAE75-E040-A249-8390-C6C592CA9991}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="untreated"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{83EFEAF9-8016-B14F-A240-1D31C677A829}" name="fish_id" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{5B1A58C4-4FA4-F040-A213-F632490B715A}" name="treatment" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{D17F91BA-89B1-6840-AC8D-3BEE4A72BE77}" name="sex" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{B386D8A1-5336-454D-B2F5-B48299CDC626}" name="start time" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{2B963070-35AB-1D41-AB37-8CD88D3AD7AB}" name="ymazeUnit" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{2A356590-AC74-5242-8339-6FCE3FFD0E34}" name="ymazePosition" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{69EE2184-8E68-0B4C-9C0D-F7E1B7B14DC2}" name="data_file_distances" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{68688BAB-7BE6-5948-8E11-EC7CCD978351}" name="data_file_zones" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{F394C5A6-BD4A-9B4D-8D1D-276E13DE473C}" name="videoFile" dataDxfId="49"/>
-    <tableColumn id="8" xr3:uid="{12BB17E8-5F27-724E-ACEA-3B58E4A5D42B}" name="Comment" dataDxfId="48"/>
-    <tableColumn id="9" xr3:uid="{97D2480A-9982-3B4C-AA40-6541F57274D0}" name="genotype" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{83EFEAF9-8016-B14F-A240-1D31C677A829}" name="fish_id" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{5B1A58C4-4FA4-F040-A213-F632490B715A}" name="treatment" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{D17F91BA-89B1-6840-AC8D-3BEE4A72BE77}" name="sex" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{B386D8A1-5336-454D-B2F5-B48299CDC626}" name="start time" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{2B963070-35AB-1D41-AB37-8CD88D3AD7AB}" name="ymazeUnit" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{2A356590-AC74-5242-8339-6FCE3FFD0E34}" name="ymazePosition" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{69EE2184-8E68-0B4C-9C0D-F7E1B7B14DC2}" name="data_file_distances" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{68688BAB-7BE6-5948-8E11-EC7CCD978351}" name="data_file_zones" dataDxfId="54"/>
+    <tableColumn id="7" xr3:uid="{F394C5A6-BD4A-9B4D-8D1D-276E13DE473C}" name="videoFile" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{12BB17E8-5F27-724E-ACEA-3B58E4A5D42B}" name="Comment" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{97D2480A-9982-3B4C-AA40-6541F57274D0}" name="genotype" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C873B688-B02F-3841-9AC9-DB63D3D6D6E4}" name="Table2" displayName="Table2" ref="A1:J60" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45">
-  <autoFilter ref="A1:J60" xr:uid="{4A127628-89D0-2941-B704-D4C232D7D28E}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{4520C07D-F5B2-3346-BFBC-BA932C91D469}" name="fish_id" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{AFB27AF1-5014-DC40-9553-64E06B3AF94E}" name="treatment" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{8C8E4483-9AAC-F143-956C-E9B7B600A9B4}" name="sex" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{6D03A179-4DD6-824E-B550-083E8863CDF7}" name="start time" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{6EDCB672-55D3-8944-979C-0FA58BC2098C}" name="ymazeUnit" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{71551E84-2AA1-7D4F-9E57-1F9B28E3EC5A}" name="ymazePosition" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{DFA66FD9-F6FB-9445-AFD7-659B23A0201C}" name="data_file"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C873B688-B02F-3841-9AC9-DB63D3D6D6E4}" name="Table2" displayName="Table2" ref="A1:L60" totalsRowShown="0" headerRowDxfId="50" headerRowBorderDxfId="49">
+  <autoFilter ref="A1:L60" xr:uid="{4A127628-89D0-2941-B704-D4C232D7D28E}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{4520C07D-F5B2-3346-BFBC-BA932C91D469}" name="fish_id" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{AFB27AF1-5014-DC40-9553-64E06B3AF94E}" name="treatment" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{8C8E4483-9AAC-F143-956C-E9B7B600A9B4}" name="sex" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{4DE3AE00-5D1D-C94E-A6B4-35DA5E23B1F9}" name="start time" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{6D03A179-4DD6-824E-B550-083E8863CDF7}" name="behavBatch" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{6EDCB672-55D3-8944-979C-0FA58BC2098C}" name="ymazeUnit" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{71551E84-2AA1-7D4F-9E57-1F9B28E3EC5A}" name="ymazePosition" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{65B46CE1-5649-9345-B0FA-0D148EE0E361}" name="data_file_distances" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{DFA66FD9-F6FB-9445-AFD7-659B23A0201C}" name="data_file_zones"/>
     <tableColumn id="8" xr3:uid="{3007FAC3-4018-0A47-8D0F-544D401DC5AD}" name="videoFile"/>
     <tableColumn id="9" xr3:uid="{9992A96B-C94F-7940-AA99-DBFF62752A53}" name="Comment"/>
-    <tableColumn id="10" xr3:uid="{E179F94A-989F-024E-BD37-1DA3BCFE2B9D}" name="genotype"/>
+    <tableColumn id="10" xr3:uid="{E179F94A-989F-024E-BD37-1DA3BCFE2B9D}" name="genotype" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1299,9 +1453,9 @@
   </sheetPr>
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G54" sqref="G54:G60"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1339,10 +1493,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
@@ -1374,13 +1528,13 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
@@ -1407,13 +1561,13 @@
         <v>2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
@@ -1440,13 +1594,13 @@
         <v>3</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
@@ -1473,20 +1627,20 @@
         <v>4</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1506,20 +1660,20 @@
         <v>5</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1539,20 +1693,20 @@
         <v>6</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1572,20 +1726,20 @@
         <v>7</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1605,20 +1759,20 @@
         <v>8</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1638,20 +1792,20 @@
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1671,20 +1825,20 @@
         <v>2</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1704,20 +1858,20 @@
         <v>3</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1737,13 +1891,13 @@
         <v>4</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="4" t="s">
@@ -1770,13 +1924,13 @@
         <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4" t="s">
@@ -1803,13 +1957,13 @@
         <v>6</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4" t="s">
@@ -1836,13 +1990,13 @@
         <v>7</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4" t="s">
@@ -1869,20 +2023,20 @@
         <v>8</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1902,13 +2056,13 @@
         <v>1</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>14</v>
@@ -1917,7 +2071,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1937,20 +2091,20 @@
         <v>2</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1970,20 +2124,20 @@
         <v>3</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2003,20 +2157,20 @@
         <v>4</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2036,20 +2190,20 @@
         <v>5</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2069,20 +2223,20 @@
         <v>6</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2102,20 +2256,20 @@
         <v>7</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2135,13 +2289,13 @@
         <v>8</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
@@ -2168,13 +2322,13 @@
         <v>1</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
@@ -2201,13 +2355,13 @@
         <v>2</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>15</v>
@@ -2236,13 +2390,13 @@
         <v>3</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4" t="s">
@@ -2269,20 +2423,20 @@
         <v>4</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2302,20 +2456,20 @@
         <v>5</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2335,20 +2489,20 @@
         <v>6</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J31" s="4"/>
       <c r="K31" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2368,20 +2522,20 @@
         <v>7</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2401,20 +2555,20 @@
         <v>8</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2434,20 +2588,20 @@
         <v>1</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2467,20 +2621,20 @@
         <v>2</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J35" s="4"/>
       <c r="K35" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2500,20 +2654,20 @@
         <v>3</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J36" s="4"/>
       <c r="K36" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2533,13 +2687,13 @@
         <v>4</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4" t="s">
@@ -2566,13 +2720,13 @@
         <v>5</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4" t="s">
@@ -2599,13 +2753,13 @@
         <v>6</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J39" s="4"/>
       <c r="K39" s="4" t="s">
@@ -2632,13 +2786,13 @@
         <v>7</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J40" s="4"/>
       <c r="K40" s="4" t="s">
@@ -2665,20 +2819,20 @@
         <v>8</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J41" s="4"/>
       <c r="K41" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2698,20 +2852,20 @@
         <v>1</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2731,20 +2885,20 @@
         <v>2</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2764,20 +2918,20 @@
         <v>3</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2797,20 +2951,20 @@
         <v>4</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2830,20 +2984,20 @@
         <v>5</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J46" s="4"/>
       <c r="K46" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2863,20 +3017,20 @@
         <v>6</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J47" s="4"/>
       <c r="K47" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2896,20 +3050,20 @@
         <v>7</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J48" s="4"/>
       <c r="K48" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2929,13 +3083,13 @@
         <v>8</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4" t="s">
@@ -2962,13 +3116,13 @@
         <v>1</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J50" s="4"/>
       <c r="K50" s="4" t="s">
@@ -2995,20 +3149,20 @@
         <v>2</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -3028,20 +3182,20 @@
         <v>3</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -3061,13 +3215,13 @@
         <v>4</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4" t="s">
@@ -3094,20 +3248,20 @@
         <v>1</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I54" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -3127,20 +3281,20 @@
         <v>2</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J55" s="4"/>
       <c r="K55" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -3160,20 +3314,20 @@
         <v>3</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H56" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J56" s="4"/>
       <c r="K56" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -3193,20 +3347,20 @@
         <v>4</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H57" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I57" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J57" s="4"/>
       <c r="K57" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -3226,20 +3380,20 @@
         <v>5</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H58" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I58" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J58" s="4"/>
       <c r="K58" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -3259,20 +3413,20 @@
         <v>6</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H59" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I59" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J59" s="4"/>
       <c r="K59" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -3292,13 +3446,13 @@
         <v>7</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H60" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I60" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J60" s="4"/>
       <c r="K60" s="4" t="s">
@@ -3325,79 +3479,79 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="E10:E17">
-    <cfRule type="cellIs" dxfId="38" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="27" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="cellIs" dxfId="36" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="31" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E42:E49">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="8" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="33" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="32" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E9">
-    <cfRule type="cellIs" dxfId="31" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18:E25">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="13" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26:E33">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="11" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E41">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="9" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50:E60">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>148</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
       <formula>139</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"het"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3420,10 +3574,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3434,13 +3589,15 @@
     <col min="4" max="4" width="11.6640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="15.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" customWidth="1"/>
-    <col min="8" max="8" width="25.1640625" customWidth="1"/>
-    <col min="9" max="9" width="35.5" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+    <col min="9" max="9" width="34.83203125" customWidth="1"/>
+    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3453,1051 +3610,2329 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5">
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
         <v>139</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5">
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
         <v>139</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5">
+      <c r="C4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
         <v>139</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5">
+      <c r="C5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
         <v>139</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
+      <c r="C6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
         <v>139</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5">
+      <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5">
         <v>139</v>
       </c>
-      <c r="F7" s="5">
+      <c r="G7" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5">
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="5">
         <v>139</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5">
+      <c r="C9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
         <v>139</v>
       </c>
-      <c r="F9" s="5">
+      <c r="G9" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5">
-        <v>148</v>
+      <c r="C10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
       </c>
       <c r="F10" s="5">
+        <v>148</v>
+      </c>
+      <c r="G10" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5">
-        <v>148</v>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
       </c>
       <c r="F11" s="5">
+        <v>148</v>
+      </c>
+      <c r="G11" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5">
-        <v>148</v>
+      <c r="C12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2</v>
       </c>
       <c r="F12" s="5">
+        <v>148</v>
+      </c>
+      <c r="G12" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5">
-        <v>148</v>
+      <c r="C13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
       </c>
       <c r="F13" s="5">
+        <v>148</v>
+      </c>
+      <c r="G13" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H13" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5">
-        <v>148</v>
+      <c r="C14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2</v>
       </c>
       <c r="F14" s="5">
+        <v>148</v>
+      </c>
+      <c r="G14" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5">
-        <v>148</v>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
       </c>
       <c r="F15" s="5">
+        <v>148</v>
+      </c>
+      <c r="G15" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H15" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5">
-        <v>148</v>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2</v>
       </c>
       <c r="F16" s="5">
+        <v>148</v>
+      </c>
+      <c r="G16" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5">
-        <v>148</v>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
       </c>
       <c r="F17" s="5">
+        <v>148</v>
+      </c>
+      <c r="G17" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5">
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3</v>
+      </c>
+      <c r="F18" s="5">
         <v>139</v>
       </c>
-      <c r="F18" s="5">
+      <c r="G18" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>70</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5">
+      <c r="C19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="5">
         <v>139</v>
       </c>
-      <c r="F19" s="5">
+      <c r="G19" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5">
+      <c r="C20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3</v>
+      </c>
+      <c r="F20" s="5">
         <v>139</v>
       </c>
-      <c r="F20" s="5">
+      <c r="G20" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5">
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E21" s="4">
+        <v>3</v>
+      </c>
+      <c r="F21" s="5">
         <v>139</v>
       </c>
-      <c r="F21" s="5">
+      <c r="G21" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5">
+      <c r="C22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
         <v>139</v>
       </c>
-      <c r="F22" s="5">
+      <c r="G22" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" t="s">
+        <v>70</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5">
+      <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E23" s="4">
+        <v>3</v>
+      </c>
+      <c r="F23" s="5">
         <v>139</v>
       </c>
-      <c r="F23" s="5">
+      <c r="G23" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5">
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E24" s="4">
+        <v>3</v>
+      </c>
+      <c r="F24" s="5">
         <v>139</v>
       </c>
-      <c r="F24" s="5">
+      <c r="G24" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>70</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5">
+      <c r="C25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="4">
+        <v>11.47</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3</v>
+      </c>
+      <c r="F25" s="5">
         <v>139</v>
       </c>
-      <c r="F25" s="5">
+      <c r="G25" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5">
-        <v>148</v>
+      <c r="C26" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4</v>
       </c>
       <c r="F26" s="5">
+        <v>148</v>
+      </c>
+      <c r="G26" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5">
-        <v>148</v>
+      <c r="C27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4</v>
       </c>
       <c r="F27" s="5">
+        <v>148</v>
+      </c>
+      <c r="G27" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5">
-        <v>148</v>
+      <c r="C28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
       </c>
       <c r="F28" s="5">
+        <v>148</v>
+      </c>
+      <c r="G28" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5">
-        <v>148</v>
+      <c r="C29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4</v>
       </c>
       <c r="F29" s="5">
+        <v>148</v>
+      </c>
+      <c r="G29" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5">
-        <v>148</v>
+      <c r="C30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E30" s="4">
+        <v>4</v>
       </c>
       <c r="F30" s="5">
+        <v>148</v>
+      </c>
+      <c r="G30" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5">
-        <v>148</v>
+      <c r="C31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E31" s="4">
+        <v>4</v>
       </c>
       <c r="F31" s="5">
+        <v>148</v>
+      </c>
+      <c r="G31" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5">
-        <v>148</v>
+      <c r="C32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E32" s="4">
+        <v>4</v>
       </c>
       <c r="F32" s="5">
+        <v>148</v>
+      </c>
+      <c r="G32" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5">
-        <v>148</v>
+      <c r="C33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="4">
+        <v>11.49</v>
+      </c>
+      <c r="E33" s="4">
+        <v>4</v>
       </c>
       <c r="F33" s="5">
+        <v>148</v>
+      </c>
+      <c r="G33" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5">
+      <c r="C34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E34" s="4">
+        <v>5</v>
+      </c>
+      <c r="F34" s="5">
         <v>139</v>
       </c>
-      <c r="F34" s="5">
+      <c r="G34" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" t="s">
+        <v>71</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5">
+      <c r="C35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E35" s="4">
+        <v>5</v>
+      </c>
+      <c r="F35" s="5">
         <v>139</v>
       </c>
-      <c r="F35" s="5">
+      <c r="G35" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35" t="s">
+        <v>71</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5">
+      <c r="C36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E36" s="4">
+        <v>5</v>
+      </c>
+      <c r="F36" s="5">
         <v>139</v>
       </c>
-      <c r="F36" s="5">
+      <c r="G36" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36" t="s">
+        <v>71</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5">
+      <c r="C37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E37" s="4">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5">
         <v>139</v>
       </c>
-      <c r="F37" s="5">
+      <c r="G37" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I37" t="s">
+        <v>55</v>
+      </c>
+      <c r="J37" t="s">
+        <v>71</v>
+      </c>
+      <c r="L37" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5">
+      <c r="C38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E38" s="4">
+        <v>5</v>
+      </c>
+      <c r="F38" s="5">
         <v>139</v>
       </c>
-      <c r="F38" s="5">
+      <c r="G38" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" t="s">
+        <v>55</v>
+      </c>
+      <c r="J38" t="s">
+        <v>71</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5">
+      <c r="C39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E39" s="4">
+        <v>5</v>
+      </c>
+      <c r="F39" s="5">
         <v>139</v>
       </c>
-      <c r="F39" s="5">
+      <c r="G39" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I39" t="s">
+        <v>55</v>
+      </c>
+      <c r="J39" t="s">
+        <v>71</v>
+      </c>
+      <c r="L39" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5">
+      <c r="C40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E40" s="4">
+        <v>5</v>
+      </c>
+      <c r="F40" s="5">
         <v>139</v>
       </c>
-      <c r="F40" s="5">
+      <c r="G40" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" t="s">
+        <v>71</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5">
+      <c r="C41" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="E41" s="4">
+        <v>5</v>
+      </c>
+      <c r="F41" s="5">
         <v>139</v>
       </c>
-      <c r="F41" s="5">
+      <c r="G41" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H41" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41" t="s">
+        <v>71</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="5">
-        <v>148</v>
+      <c r="C42" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E42" s="4">
+        <v>6</v>
       </c>
       <c r="F42" s="5">
+        <v>148</v>
+      </c>
+      <c r="G42" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J42" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L42" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5">
-        <v>148</v>
+      <c r="C43" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E43" s="4">
+        <v>6</v>
       </c>
       <c r="F43" s="5">
+        <v>148</v>
+      </c>
+      <c r="G43" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="5">
-        <v>148</v>
+      <c r="C44" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E44" s="4">
+        <v>6</v>
       </c>
       <c r="F44" s="5">
+        <v>148</v>
+      </c>
+      <c r="G44" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L44" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="5">
-        <v>148</v>
+      <c r="C45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E45" s="4">
+        <v>6</v>
       </c>
       <c r="F45" s="5">
+        <v>148</v>
+      </c>
+      <c r="G45" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L45" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="5">
-        <v>148</v>
+      <c r="C46" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E46" s="4">
+        <v>6</v>
       </c>
       <c r="F46" s="5">
+        <v>148</v>
+      </c>
+      <c r="G46" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H46" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="5">
-        <v>148</v>
+      <c r="C47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D47" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E47" s="4">
+        <v>6</v>
       </c>
       <c r="F47" s="5">
+        <v>148</v>
+      </c>
+      <c r="G47" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="5">
-        <v>148</v>
+      <c r="C48" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E48" s="4">
+        <v>6</v>
       </c>
       <c r="F48" s="5">
+        <v>148</v>
+      </c>
+      <c r="G48" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="5">
-        <v>148</v>
+      <c r="C49" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="4">
+        <v>13.01</v>
+      </c>
+      <c r="E49" s="4">
+        <v>6</v>
       </c>
       <c r="F49" s="5">
+        <v>148</v>
+      </c>
+      <c r="G49" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H49" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="5">
+      <c r="C50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="E50" s="4">
+        <v>7</v>
+      </c>
+      <c r="F50" s="5">
         <v>139</v>
       </c>
-      <c r="F50" s="5">
+      <c r="G50" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H50" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I50" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J50" t="s">
+        <v>72</v>
+      </c>
+      <c r="L50" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="5">
+      <c r="C51" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="E51" s="4">
+        <v>7</v>
+      </c>
+      <c r="F51" s="5">
         <v>139</v>
       </c>
-      <c r="F51" s="5">
+      <c r="G51" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H51" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I51" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J51" t="s">
+        <v>72</v>
+      </c>
+      <c r="L51" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="5">
+      <c r="C52" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="E52" s="4">
+        <v>7</v>
+      </c>
+      <c r="F52" s="5">
         <v>139</v>
       </c>
-      <c r="F52" s="5">
+      <c r="G52" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H52" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J52" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="5">
+      <c r="C53" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="4">
+        <v>14.05</v>
+      </c>
+      <c r="E53" s="4">
+        <v>7</v>
+      </c>
+      <c r="F53" s="5">
         <v>139</v>
       </c>
-      <c r="F53" s="5">
+      <c r="G53" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H53" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J53" t="s">
+        <v>72</v>
+      </c>
+      <c r="L53" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="5">
-        <v>148</v>
+      <c r="C54" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>8</v>
       </c>
       <c r="F54" s="5">
+        <v>148</v>
+      </c>
+      <c r="G54" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="5">
-        <v>148</v>
+      <c r="C55" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E55" s="4">
+        <v>8</v>
       </c>
       <c r="F55" s="5">
+        <v>148</v>
+      </c>
+      <c r="G55" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H55" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L55" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5">
-        <v>148</v>
+      <c r="C56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D56" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E56" s="4">
+        <v>8</v>
       </c>
       <c r="F56" s="5">
+        <v>148</v>
+      </c>
+      <c r="G56" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="5">
-        <v>148</v>
+      <c r="C57" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D57" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E57" s="4">
+        <v>8</v>
       </c>
       <c r="F57" s="5">
+        <v>148</v>
+      </c>
+      <c r="G57" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H57" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L57" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5">
-        <v>148</v>
+      <c r="C58" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D58" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E58" s="4">
+        <v>8</v>
       </c>
       <c r="F58" s="5">
+        <v>148</v>
+      </c>
+      <c r="G58" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H58" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J58" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="5">
-        <v>148</v>
+      <c r="C59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D59" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E59" s="4">
+        <v>8</v>
       </c>
       <c r="F59" s="5">
+        <v>148</v>
+      </c>
+      <c r="G59" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H59" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J59" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L59" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="5">
-        <v>148</v>
+      <c r="C60" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="4">
+        <v>14.1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>8</v>
       </c>
       <c r="F60" s="5">
+        <v>148</v>
+      </c>
+      <c r="G60" s="5">
         <v>7</v>
       </c>
+      <c r="H60" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I60" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J60" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L60" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
+  <conditionalFormatting sqref="F10:F17">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42:F49">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F25">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F26:F33">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F34:F41">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F50:F60">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>148</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>139</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+  <conditionalFormatting sqref="L1">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"het"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E17">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
-      <formula>148</formula>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"het"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
-      <formula>139</formula>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"hom"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:E49">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18:E25">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E33">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34:E41">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50:E60">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>148</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>139</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="http://192.168.1.139/zantiks/media/YMaze_tracking-20230613T104021-f30.avi" xr:uid="{C2FADB0B-AC87-4C42-B9B8-68C51E2796F6}"/>
+    <hyperlink ref="J3:J9" r:id="rId2" display="http://192.168.1.139/zantiks/media/YMaze_tracking-20230613T104021-f30.avi" xr:uid="{E9D7FE20-8C0C-6A4E-BA0E-CDC03543174D}"/>
+    <hyperlink ref="H2" r:id="rId3" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{88EB24CD-C59C-8A4C-96D5-C49CA4A214EF}"/>
+    <hyperlink ref="I2" r:id="rId4" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{DCE61C78-9BD2-3144-A4FF-9886FA762741}"/>
+    <hyperlink ref="H18" r:id="rId5" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{0B1A56C9-0DF4-B744-BCAA-E4FBE42E36E4}"/>
+    <hyperlink ref="I18" r:id="rId6" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{4D3EAC93-7DBB-0247-98A1-E0AA5CEA37E9}"/>
+    <hyperlink ref="H34" r:id="rId7" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{1CB90C26-1BBD-034E-9DF6-DE3213CCA4DF}"/>
+    <hyperlink ref="I50" r:id="rId8" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141129.csv" xr:uid="{6F51DF54-9BB5-944F-A084-AD035765AFEA}"/>
+    <hyperlink ref="H50" r:id="rId9" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141130-data_totals.csv" xr:uid="{6F7D2766-2042-344E-9BA3-97663621E8D0}"/>
+    <hyperlink ref="H3" r:id="rId10" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{A796C279-9516-D840-B7F1-26C059C6958A}"/>
+    <hyperlink ref="H4" r:id="rId11" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{C4548F46-F0C9-EF4B-B8D4-A4176C018F2A}"/>
+    <hyperlink ref="H5" r:id="rId12" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{2FB27EB2-4911-4B4A-BB36-B8D40C917FBE}"/>
+    <hyperlink ref="H6" r:id="rId13" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{2A473E96-9485-A944-B72D-6719DC26758B}"/>
+    <hyperlink ref="H7" r:id="rId14" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{67DEFD64-71BC-CF42-B034-589FD8FA32C2}"/>
+    <hyperlink ref="H8" r:id="rId15" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{6E925D8A-A510-ED4D-AFB3-5C47B9FE066B}"/>
+    <hyperlink ref="H9" r:id="rId16" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103951-data_totals.csv" xr:uid="{787ACCD9-BEFA-C642-B2D5-3EBCF5354357}"/>
+    <hyperlink ref="I3" r:id="rId17" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{31B771C8-C32B-8D4D-A510-FFE37718EC84}"/>
+    <hyperlink ref="I4" r:id="rId18" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{0F8F4BF0-0261-EA40-A702-E937FC769F6B}"/>
+    <hyperlink ref="I5" r:id="rId19" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{C447367F-9534-5C4E-833E-4D7B244CCC46}"/>
+    <hyperlink ref="I6" r:id="rId20" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{DA5BCDAE-E76B-BE4D-9B28-6331D43A129B}"/>
+    <hyperlink ref="I7" r:id="rId21" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{000AC4DE-6732-7643-8977-A76FB76BD8FA}"/>
+    <hyperlink ref="I8" r:id="rId22" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{6C030420-A3BF-E541-A627-A50CD77F88E5}"/>
+    <hyperlink ref="I9" r:id="rId23" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T103950.csv" xr:uid="{73BB56D3-76F0-A84D-94E3-FB6012E30738}"/>
+    <hyperlink ref="H19" r:id="rId24" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{5E107465-04C7-9D4E-AA7D-9A045BE7C539}"/>
+    <hyperlink ref="H20" r:id="rId25" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{5750CA92-2C46-E841-8A3F-C2810652C38E}"/>
+    <hyperlink ref="H21" r:id="rId26" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{F7FC0B50-A6CF-794E-9E80-7D7C9C4FBFCE}"/>
+    <hyperlink ref="H22" r:id="rId27" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{44625FF9-BA71-C54E-8522-3390BC114D59}"/>
+    <hyperlink ref="H23" r:id="rId28" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{E339759B-4ECD-EB4E-A28C-98C5F8B5179F}"/>
+    <hyperlink ref="H24" r:id="rId29" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{720A67C1-7812-7D49-B196-B501FFE58344}"/>
+    <hyperlink ref="H25" r:id="rId30" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104-data_totals.csv" xr:uid="{98774AA5-63EF-5240-9631-8835CF594F41}"/>
+    <hyperlink ref="I19" r:id="rId31" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{4EB25B14-8CEE-5D43-AE1E-A71BEC07522A}"/>
+    <hyperlink ref="I20" r:id="rId32" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{3718F819-C71F-2B47-90D1-72223C7E690C}"/>
+    <hyperlink ref="I21" r:id="rId33" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{4E1E47C4-CBE1-7942-80B5-626333384538}"/>
+    <hyperlink ref="I22" r:id="rId34" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{9F82A998-CFB2-3445-9E41-AA49BB3DCAA1}"/>
+    <hyperlink ref="I23" r:id="rId35" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{D19A554F-0457-6F4A-AACC-70E5B84F77A3}"/>
+    <hyperlink ref="I24" r:id="rId36" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{8A96D694-8341-1F4D-9A63-61A077C0A2FD}"/>
+    <hyperlink ref="I25" r:id="rId37" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T115104.csv" xr:uid="{E029ACF6-62A6-114A-B055-D173D52969C4}"/>
+    <hyperlink ref="H35" r:id="rId38" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{CADB990D-A6C1-7E42-A1B5-0BF0C5C49DAA}"/>
+    <hyperlink ref="H36" r:id="rId39" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{1DC87125-620A-E947-B0B1-68938495C126}"/>
+    <hyperlink ref="H37" r:id="rId40" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{3696077D-2FDC-3244-BA82-96D7CD98AE20}"/>
+    <hyperlink ref="H38" r:id="rId41" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{ECA24EF1-99DE-0D4D-916E-075AB20B8B70}"/>
+    <hyperlink ref="H39" r:id="rId42" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{E820E15B-A973-EE4D-9B1D-9394982134C5}"/>
+    <hyperlink ref="H40" r:id="rId43" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{93B443D6-7252-3847-A166-BE9B016E6B28}"/>
+    <hyperlink ref="H41" r:id="rId44" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T130222-data_totals.csv" xr:uid="{8CAAEAD3-CC32-3F42-A531-A98ECA53630A}"/>
+    <hyperlink ref="I51" r:id="rId45" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141129.csv" xr:uid="{CEFDECC3-8112-544E-95CC-39ACDF697BB6}"/>
+    <hyperlink ref="I52" r:id="rId46" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141129.csv" xr:uid="{13CFEB3E-3FD0-9142-ADE0-7877AA9444C2}"/>
+    <hyperlink ref="I53" r:id="rId47" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141129.csv" xr:uid="{F7BC38C2-F1A0-5340-B7B6-ECAD2534C21A}"/>
+    <hyperlink ref="H51" r:id="rId48" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141130-data_totals.csv" xr:uid="{9E413BD0-796C-954B-ACF9-99837378144E}"/>
+    <hyperlink ref="H52" r:id="rId49" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141130-data_totals.csv" xr:uid="{6D935732-273F-5742-93A4-845E0041CD8B}"/>
+    <hyperlink ref="H53" r:id="rId50" display="http://192.168.1.139/zantiks/logs/ymaze_inLT-20230613T141130-data_totals.csv" xr:uid="{6C60FAEF-A24A-AC47-A214-74F8281D0C6B}"/>
+    <hyperlink ref="J10" r:id="rId51" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{A4AE1FEE-C9B5-0F4E-B0B8-416A8769FEEF}"/>
+    <hyperlink ref="J26" r:id="rId52" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{7FA507A7-260A-3E43-B3B4-947690275BCA}"/>
+    <hyperlink ref="J54" r:id="rId53" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{8FD66116-CC5D-8E43-831C-692BECF93BCA}"/>
+    <hyperlink ref="H10" r:id="rId54" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{69D54611-808C-2F43-A11B-1DF167E7A0B8}"/>
+    <hyperlink ref="I10" r:id="rId55" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{AB0EF440-97DA-BF44-9D99-A20285943A40}"/>
+    <hyperlink ref="H26" r:id="rId56" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{996B5E43-9963-A24B-82FD-895DDCFE72A3}"/>
+    <hyperlink ref="I26" r:id="rId57" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{3810DCA5-8006-E04F-BD81-E75DF18837F3}"/>
+    <hyperlink ref="I42" r:id="rId58" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{79945D09-00B3-6241-85B5-332A1E36D4F2}"/>
+    <hyperlink ref="H54" r:id="rId59" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{60D34827-0DCB-2C4B-A215-5EF8B2B9062C}"/>
+    <hyperlink ref="I54" r:id="rId60" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{A14A2A4D-08B9-374D-A46A-8242197B681C}"/>
+    <hyperlink ref="J11" r:id="rId61" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{CBE58507-9F06-F841-8B63-D20AF580524F}"/>
+    <hyperlink ref="J12" r:id="rId62" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{33C9421D-ACAC-E342-8AB7-615AC3A683EE}"/>
+    <hyperlink ref="J13" r:id="rId63" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{4AE9CE47-228D-B94A-AABC-40CD6AAF0137}"/>
+    <hyperlink ref="J14" r:id="rId64" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{B957D8B5-05C8-B546-85F6-1D9FD4D8FD21}"/>
+    <hyperlink ref="J15" r:id="rId65" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{6C531CE4-DE97-C942-8F99-3C7B8A1B11C1}"/>
+    <hyperlink ref="J16" r:id="rId66" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{8938CBAC-ADCA-C343-817A-F96F47E42E6B}"/>
+    <hyperlink ref="J17" r:id="rId67" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T104205-f30.avi" xr:uid="{F4AE7536-F2BD-8047-8B91-63F4B140C2CD}"/>
+    <hyperlink ref="H11" r:id="rId68" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{6123FCBB-C966-9045-8571-F6364534F14B}"/>
+    <hyperlink ref="H12" r:id="rId69" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{66F0FD94-B1A3-DB49-8FD2-1A6D2B6EA7FD}"/>
+    <hyperlink ref="H13" r:id="rId70" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{D3EFD28A-97EF-9147-8C90-A55D8F88AD90}"/>
+    <hyperlink ref="H14" r:id="rId71" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{B7168110-C720-5748-8913-191EF5317B23}"/>
+    <hyperlink ref="H15" r:id="rId72" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{C11269FB-0B83-B747-A29E-571A8E24E0D9}"/>
+    <hyperlink ref="H16" r:id="rId73" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{6CE3C8B9-F0D7-3241-85F8-010B398927C6}"/>
+    <hyperlink ref="H17" r:id="rId74" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104135-data_totals.csv" xr:uid="{440E5887-D012-1243-A2B4-205B0C0BB8FE}"/>
+    <hyperlink ref="I11" r:id="rId75" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{C12903B2-8268-5347-AEE7-7BC8714D0245}"/>
+    <hyperlink ref="I12" r:id="rId76" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{A169C35F-E957-5844-B5D0-816B9DBADD39}"/>
+    <hyperlink ref="I13" r:id="rId77" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{DA0218C3-D4D6-8940-BB22-969A35B9DF49}"/>
+    <hyperlink ref="I14" r:id="rId78" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{9538B696-615A-0B45-B7D1-E4269B60E83B}"/>
+    <hyperlink ref="I15" r:id="rId79" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{777F8AB0-3042-2442-888A-E7AF92F67E45}"/>
+    <hyperlink ref="I16" r:id="rId80" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{0630522A-79B6-E348-9D03-2C381583F0CE}"/>
+    <hyperlink ref="I17" r:id="rId81" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T104134.csv" xr:uid="{9DB80527-E6FF-9E49-8468-ABC4EF5A428C}"/>
+    <hyperlink ref="J27" r:id="rId82" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{D6D5EA25-E60B-7840-9C65-BD1A6832A057}"/>
+    <hyperlink ref="J28" r:id="rId83" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{7164B63B-043E-E640-AEEB-E41CD9688573}"/>
+    <hyperlink ref="J29" r:id="rId84" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{C7DDE830-B5A0-F749-A4FA-2FF2CEB24873}"/>
+    <hyperlink ref="J30" r:id="rId85" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{37F8AB11-7F8B-6243-9C76-D636218B0050}"/>
+    <hyperlink ref="J31" r:id="rId86" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{C7C78599-57A6-794B-ADF7-957A076FD0D6}"/>
+    <hyperlink ref="J32" r:id="rId87" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{2B69D476-85E6-B447-9CEB-7194A18374A8}"/>
+    <hyperlink ref="J33" r:id="rId88" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T115329-f30.avi" xr:uid="{BB92B446-84EB-DE46-A642-11901CB09D46}"/>
+    <hyperlink ref="H27" r:id="rId89" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{8851D7D6-94B4-A246-9A85-34553B3495B8}"/>
+    <hyperlink ref="H28" r:id="rId90" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{D6BDD7A5-6C37-2A44-A600-1B7143EBAED9}"/>
+    <hyperlink ref="H29" r:id="rId91" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{1021BFA4-2720-6640-B8E7-93BB4AAFEE35}"/>
+    <hyperlink ref="H30" r:id="rId92" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{CD41E07E-BC72-4848-AED3-1AD95EEA9B68}"/>
+    <hyperlink ref="H31" r:id="rId93" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{05AC6ACF-9A8C-8344-B67C-1E4A23ABB856}"/>
+    <hyperlink ref="H32" r:id="rId94" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{3E3ACEE5-9F9D-EF45-9FBA-4A0E0453B486}"/>
+    <hyperlink ref="H33" r:id="rId95" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258-data_totals.csv" xr:uid="{2281543C-ABDB-5A4C-9D50-F41EFB2516C9}"/>
+    <hyperlink ref="I27" r:id="rId96" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{D34A4805-E0E6-FE4C-B7A9-DC3B91E14B2A}"/>
+    <hyperlink ref="I28" r:id="rId97" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{D3F9BCF6-7B83-D845-85C0-E9A351AC7869}"/>
+    <hyperlink ref="I29" r:id="rId98" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{A079B471-0CDF-C640-9812-39AFDBF19D76}"/>
+    <hyperlink ref="I30" r:id="rId99" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{B0461DA6-27BE-E242-9DCA-CB273A650FFE}"/>
+    <hyperlink ref="I31" r:id="rId100" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{06AADB15-D5D6-C441-8B2A-82D001D3A2E2}"/>
+    <hyperlink ref="I32" r:id="rId101" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{C019F3F7-4AE1-204C-897E-6FB3B4702CBA}"/>
+    <hyperlink ref="I33" r:id="rId102" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T115258.csv" xr:uid="{420A479F-6783-744B-9612-9A5C3CC7FF7F}"/>
+    <hyperlink ref="J43" r:id="rId103" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{89A3325D-ADDE-C942-8939-793D4F8B1635}"/>
+    <hyperlink ref="J44" r:id="rId104" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{E8786C72-0434-A84D-87FF-08E231FE59DB}"/>
+    <hyperlink ref="J45" r:id="rId105" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{1865C4FB-9E1B-B54C-AB8B-ADE308B93ED5}"/>
+    <hyperlink ref="J46" r:id="rId106" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{61D647A8-35D9-AD47-A79B-AFACB8FF4B97}"/>
+    <hyperlink ref="J47" r:id="rId107" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{6D663969-B839-1C41-AEE2-E69FEB5B48EA}"/>
+    <hyperlink ref="J48" r:id="rId108" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{83336E58-1A5F-BC4C-A481-09234EAEC948}"/>
+    <hyperlink ref="J49" r:id="rId109" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{867ADA35-654B-9A47-AFBE-32B9FE09EE8E}"/>
+    <hyperlink ref="I43" r:id="rId110" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{8E25FDD3-EA90-0940-9908-F1D6F72E64A6}"/>
+    <hyperlink ref="I44" r:id="rId111" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{BC1F0178-E4D9-8641-B185-15C50A4E9585}"/>
+    <hyperlink ref="I45" r:id="rId112" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{D5548E4D-1208-4744-89A4-B7CFDC688C61}"/>
+    <hyperlink ref="I46" r:id="rId113" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{E5EA55BA-8A71-8B47-BB2B-D553D0AB06B5}"/>
+    <hyperlink ref="I47" r:id="rId114" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{1CB07BD1-37C5-F442-AA8B-6370716637BC}"/>
+    <hyperlink ref="I48" r:id="rId115" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{A24D301C-5956-914F-BC19-A87B658EF3A3}"/>
+    <hyperlink ref="I49" r:id="rId116" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T130502.csv" xr:uid="{726EC93E-FFFB-D249-9FA0-C3C7D7292DE4}"/>
+    <hyperlink ref="J55" r:id="rId117" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{64F745B2-9278-FC46-B882-C9A529BE663B}"/>
+    <hyperlink ref="J56" r:id="rId118" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{3795260B-51BB-DF4D-8F20-8EFA6BBE05F3}"/>
+    <hyperlink ref="J57" r:id="rId119" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{C31F400F-54AF-7241-8755-34DB159BF1A2}"/>
+    <hyperlink ref="J58" r:id="rId120" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{39AB0439-271E-694A-B19A-3A0F865E1E69}"/>
+    <hyperlink ref="J59" r:id="rId121" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{327EACA4-B7A5-BB4D-995C-0E9176C33C57}"/>
+    <hyperlink ref="J60" r:id="rId122" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T141400-f30.avi" xr:uid="{93917B40-CC4D-1B41-A07F-3A731422A912}"/>
+    <hyperlink ref="H55" r:id="rId123" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{32C28ADC-8503-4E40-BA22-9E4CFB96E6F2}"/>
+    <hyperlink ref="H56" r:id="rId124" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{15230229-509B-D34E-8B49-FF811FBD2502}"/>
+    <hyperlink ref="H57" r:id="rId125" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{57288F60-E89F-1E4F-BC48-CD05503B87BC}"/>
+    <hyperlink ref="H58" r:id="rId126" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{A5B70F27-0DEA-B744-8A04-1D311C181018}"/>
+    <hyperlink ref="H59" r:id="rId127" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{902E0F0C-4CE3-9349-9441-3F411C4E530E}"/>
+    <hyperlink ref="H60" r:id="rId128" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141330-data_totals.csv" xr:uid="{2F7A6E0C-9B4B-DA40-AC6D-535140AFFF6B}"/>
+    <hyperlink ref="I55" r:id="rId129" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{A45A6003-11CF-234E-B418-4B6384B879DD}"/>
+    <hyperlink ref="I56" r:id="rId130" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{2993620B-97CA-864E-8099-BD76C3844C5A}"/>
+    <hyperlink ref="I57" r:id="rId131" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{BF921094-BF06-E34D-A5BF-296C9F9CBCCA}"/>
+    <hyperlink ref="I58" r:id="rId132" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{AFD4793F-74D5-4A47-A59A-2C8242718474}"/>
+    <hyperlink ref="I59" r:id="rId133" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{58225382-41B9-8647-9731-EE48729846B8}"/>
+    <hyperlink ref="I60" r:id="rId134" display="http://192.168.1.148/zantiks/logs/ymazeinLT-20230613T141329.csv" xr:uid="{5FE2CF60-EEBE-5145-99FE-B185445543DA}"/>
+    <hyperlink ref="J42" r:id="rId135" display="http://192.168.1.148/zantiks/media/YMaze_tracking-20230613T130533-f30.avi" xr:uid="{33718896-5BF6-3947-84F9-5B3A4AD88C84}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId136"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>